<commit_message>
Fixed Main Table Element
</commit_message>
<xml_diff>
--- a/placementInfovitians02021.xlsx
+++ b/placementInfovitians02021.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,6 +1143,1333 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Leadsquared</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5 LPA fixed +2 LPA variable performance-based</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>HealthPlix Technologies</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>- 6lpa (3lpa fixed, completion of 12 months 1-month extra salary</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Paragon Digital Services</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>3 LPA</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Marlabs</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>3.5 LPA</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Viacom 18</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>8 LPA</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KHOJ</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2 LPA</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Eaton</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>10 LPA</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BoardInfinity</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BoardInfinity</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>5-6 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Mantra Technologies</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Pin Click</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4.8 LPA (3 LPA fixed + 1.8 LPA Variable)</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Treebo Hotels</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Sandvine</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Super Dream</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>14,70,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Sandvine Technologies</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>14.7 LPA</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Extramarks</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>8 LPA</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Hexaview Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Application Engineer – Regular offer
+  Member of Technical Staff - Dream offer</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>4 LPA - Application Engineer
+6 LPA - Member of Technical Staff</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>People Interactive (India) Private Limited</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>11 LPA</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>McKinsey</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>8.8 LPA + Benefits</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Zoho Corporation</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Online Test: 14.02.2021
+Selection Process :17.02.2021</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>·  6.5L Offer - Candidates those who clear all levels of tests and interviews.
+·  4.6L Offer - Candidates who fell short of the expectations, but meet our requirements.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Weir EnSci</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Dream core</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>4 LPA</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ConvertCart</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Sales Analyst - 5 fixed + 3 Variable (8 LPA)
+Business Analyst - 4 Fixed + 4 Variable  (8 LPA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Tata Communications</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>6.5 LPA</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Godrej and Boyce</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>6 LPA after Conversion</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Leadsquared</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>5 LPA fixed +2 LPA variable performance-based</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>HealthPlix Technologies</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>- 6lpa (3lpa fixed, completion of 12 months 1-month extra salary</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Paragon Digital Services</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>3 LPA</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Marlabs</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>3.5 LPA</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Viacom 18</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>8 LPA</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>KHOJ</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2 LPA</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Eaton</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>10 LPA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BoardInfinity</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>BoardInfinity</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>5-6 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Mantra Technologies</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Pin Click</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>4.8 LPA (3 LPA fixed + 1.8 LPA Variable)</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Treebo Hotels</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>5 LPA</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Sandvine</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Super Dream</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>14,70,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sandvine Technologies</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>14.7 LPA</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Extramarks</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>8 LPA</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Hexaview Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Application Engineer – Regular offer
+  Member of Technical Staff - Dream offer</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>4 LPA - Application Engineer
+6 LPA - Member of Technical Staff</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>People Interactive (India) Private Limited</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Super Dream software</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>11 LPA</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>McKinsey</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>8.8 LPA + Benefits</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Zoho Corporation</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Online Test: 14.02.2021
+Selection Process :17.02.2021</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>·  6.5L Offer - Candidates those who clear all levels of tests and interviews.
+·  4.6L Offer - Candidates who fell short of the expectations, but meet our requirements.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Weir EnSci</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Dream core</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>4 LPA</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ConvertCart</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Sales Analyst - 5 fixed + 3 Variable (8 LPA)
+Business Analyst - 4 Fixed + 4 Variable  (8 LPA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Tata Communications</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>6.5 LPA</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Godrej and Boyce</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Dream</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>6 LPA after Conversion</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Haasyl</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>6 LPA</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Royal Enfield</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Dream software</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Etech Global Services</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2 LPA</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>PopcornApps</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2.2 LPA</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>HCL</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Regular software</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Will be announced later</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>